<commit_message>
Testing by Siva - 19Sep17
Testing by Siva - 19Sep17
</commit_message>
<xml_diff>
--- a/ApplyEvent_For_UnitsInVerificationZone/Release Documents/Testing - Apply Billable Event for Units in Verification Zone.xlsx
+++ b/ApplyEvent_For_UnitsInVerificationZone/Release Documents/Testing - Apply Billable Event for Units in Verification Zone.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Praveen\Documents\GitHub\DPW_Caucedo\Release Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11595" xr2:uid="{C4B5B8C0-2545-4D32-B0BC-40ABCBAA045E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Client Requirement" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="124519"/>
   <fileRecoveryPr autoRecover="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="109">
   <si>
     <t>Case Desc</t>
   </si>
@@ -63,9 +58,6 @@
   </si>
   <si>
     <t>DataVal1</t>
-  </si>
-  <si>
-    <t>DataVal2</t>
   </si>
   <si>
     <t>Actual Result</t>
@@ -282,15 +274,6 @@
   </si>
   <si>
     <t>1. Select an Import unit with following criteria
-  a. V-State : other than Active
-  b. T-State : “Yard”
-  c. Grp ID : Configured in Gen Ref
-  d. Position : Configured in Gen Ref
-  e. Freight Kind = FCL/LCL/MTY
-2. Execute the Groovy Job once</t>
-  </si>
-  <si>
-    <t>1. Select an Import unit with following criteria
   a. V-State : “Active”  
   b. T-State : “Yard”
   c. Grp ID : Configured in Gen Ref
@@ -451,12 +434,152 @@
     <t>1)  Observe Event “NSWVERIF” recorded &amp; Event Notes with Grp ID &amp; Yard Block Name for Import, Full, Active units exist in configured verification Zone
 2) Other units are not updated</t>
   </si>
+  <si>
+    <t>HJMU1542797</t>
+  </si>
+  <si>
+    <t>AMFU2003595</t>
+  </si>
+  <si>
+    <t>MRKU1036660</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Yard</t>
+  </si>
+  <si>
+    <t>CVD</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>DataVal3</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>MRKU4365090</t>
+  </si>
+  <si>
+    <t>ZR</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>1. Select an Import unit with following criteria
+  a. V-State : Active
+  b. T-State : other than “Yard”
+  c. Grp ID : Configured in Gen Ref
+  d. Position : Configured in Gen Ref
+  e. Freight Kind = FCL/LCL/MTY
+2. Execute the Groovy Job once</t>
+  </si>
+  <si>
+    <t>yard</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>CCLU7004720</t>
+  </si>
+  <si>
+    <t>ECMU9436179</t>
+  </si>
+  <si>
+    <t>DC,FL</t>
+  </si>
+  <si>
+    <t>MEDU1415597</t>
+  </si>
+  <si>
+    <t>C.117.G.2</t>
+  </si>
+  <si>
+    <t>PIT / C.117.G.2</t>
+  </si>
+  <si>
+    <t>FL,ZR</t>
+  </si>
+  <si>
+    <t>MRKU4365090, MSKU6190080</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>HN</t>
+  </si>
+  <si>
+    <t>VH</t>
+  </si>
+  <si>
+    <t>HN, AW</t>
+  </si>
+  <si>
+    <t>1)  Observed Event “NSWVERIF” recorded in Unit 
+2) Event Notes with Grp ID &amp; Yard Block Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  Observed Event “NSWVERIF” not recorded in Unit </t>
+  </si>
+  <si>
+    <t>1)  Observed Event “NSWVERIF” recorded in Units
+2) Event Notes with Grp ID &amp; Yard Block Name</t>
+  </si>
+  <si>
+    <t>VH, CVD</t>
+  </si>
+  <si>
+    <t>DC,FL,VH,CVD</t>
+  </si>
+  <si>
+    <t>MSKU6190080, MRKU1036660</t>
+  </si>
+  <si>
+    <t>TGHU8098009, MSKU6190080, MRKU1036660</t>
+  </si>
+  <si>
+    <t>ZR, VH, CVD</t>
+  </si>
+  <si>
+    <t>Inbound / Yard</t>
+  </si>
+  <si>
+    <t>Inbound</t>
+  </si>
+  <si>
+    <t>HJMU1542797,TGHU8098009, MSKU6190080, MRKU1036660</t>
+  </si>
+  <si>
+    <t>TGHU8098009,  MSKU6190080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Billable Event to Single or multiple Import- Full container recieved via Truck Transaction &amp; Active unit exist in configured verification Zone </t>
+  </si>
+  <si>
+    <t>MSCU6551650</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -886,6 +1009,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,7 +1076,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -999,7 +1128,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1193,34 +1322,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AAD4A7-07F2-451A-8A95-73A47381865C}">
-  <dimension ref="A1:N25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.140625" style="1" customWidth="1"/>
-    <col min="5" max="11" width="4" style="2" customWidth="1"/>
-    <col min="12" max="12" width="44" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="36.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="12" width="4" style="2" customWidth="1"/>
+    <col min="13" max="13" width="44" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="36.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="20"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -1233,17 +1362,18 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
-      <c r="M1" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" s="37"/>
-    </row>
-    <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="M1" s="21"/>
+      <c r="N1" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="37"/>
+    </row>
+    <row r="2" spans="1:15" ht="23.25">
       <c r="A2" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -1255,15 +1385,16 @@
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M2" s="18"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -1275,10 +1406,11 @@
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="39"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M3" s="18"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="39"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="23"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -1291,10 +1423,11 @@
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
       <c r="L4" s="19"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="41"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="19"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="41"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="24"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -1309,14 +1442,15 @@
       <c r="J5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="12"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="12"/>
-      <c r="N5" s="25"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+      <c r="N5" s="12"/>
+      <c r="O5" s="25"/>
+    </row>
+    <row r="6" spans="1:15" s="3" customFormat="1" ht="39">
       <c r="A6" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -1346,443 +1480,808 @@
         <v>11</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="O6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" ht="105">
       <c r="A7" s="28">
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="29"/>
-    </row>
-    <row r="8" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="E7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="29"/>
+    </row>
+    <row r="8" spans="1:15" ht="105">
       <c r="A8" s="28">
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="29"/>
-    </row>
-    <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" s="29"/>
+    </row>
+    <row r="9" spans="1:15" ht="105">
       <c r="A9" s="28">
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="29"/>
-    </row>
-    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O9" s="29"/>
+    </row>
+    <row r="10" spans="1:15" ht="105">
       <c r="A10" s="28">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="29"/>
-    </row>
-    <row r="11" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="J10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O10" s="29"/>
+    </row>
+    <row r="11" spans="1:15" ht="105">
       <c r="A11" s="28">
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="29"/>
-    </row>
-    <row r="12" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="L11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="29"/>
+    </row>
+    <row r="12" spans="1:15" ht="105">
       <c r="A12" s="28">
         <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="29"/>
-    </row>
-    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="29"/>
+    </row>
+    <row r="13" spans="1:15" ht="105">
       <c r="A13" s="28">
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="29"/>
-    </row>
-    <row r="14" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="L13" s="11"/>
+      <c r="M13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O13" s="29"/>
+    </row>
+    <row r="14" spans="1:15" ht="120">
       <c r="A14" s="28">
         <v>8</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="29"/>
-    </row>
-    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O14" s="29"/>
+    </row>
+    <row r="15" spans="1:15" ht="120">
       <c r="A15" s="28">
         <v>9</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="29"/>
-    </row>
-    <row r="16" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="L15" s="11"/>
+      <c r="M15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" s="29"/>
+    </row>
+    <row r="16" spans="1:15" ht="135">
+      <c r="A16" s="42">
         <v>10</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>38</v>
+      <c r="B16" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="29"/>
-    </row>
-    <row r="17" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O16" s="29"/>
+    </row>
+    <row r="17" spans="1:15" ht="105">
       <c r="A17" s="28">
         <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="29"/>
-    </row>
-    <row r="18" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O17" s="29"/>
+    </row>
+    <row r="18" spans="1:15" ht="120">
       <c r="A18" s="28">
         <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="29"/>
-    </row>
-    <row r="19" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="E18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O18" s="29"/>
+    </row>
+    <row r="19" spans="1:15" ht="141.75">
       <c r="A19" s="28">
         <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>91</v>
+      </c>
       <c r="K19" s="11"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="29"/>
-    </row>
-    <row r="20" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="L19" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="29"/>
+    </row>
+    <row r="20" spans="1:15" ht="141.75">
       <c r="A20" s="28">
         <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="29"/>
-    </row>
-    <row r="21" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O20" s="29"/>
+    </row>
+    <row r="21" spans="1:15" ht="141.75">
       <c r="A21" s="28">
         <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="D21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="29"/>
-    </row>
-    <row r="22" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="K21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O21" s="29"/>
+    </row>
+    <row r="22" spans="1:15" ht="211.5">
       <c r="A22" s="28">
         <v>16</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="29"/>
-    </row>
-    <row r="23" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" ht="279.75">
       <c r="A23" s="28">
         <v>17</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="29"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="29"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O23" s="29"/>
+    </row>
+    <row r="24" spans="1:15" ht="105">
+      <c r="A24" s="28">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O24" s="29"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1">
       <c r="A25" s="30"/>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -1794,76 +2293,77 @@
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
-      <c r="L25" s="31"/>
+      <c r="L25" s="32"/>
       <c r="M25" s="31"/>
-      <c r="N25" s="33"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="M1:N4"/>
+    <mergeCell ref="N1:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B63A24-EE73-4474-940E-4AE7306C3821}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="9"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="9"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>